<commit_message>
Made a tidy rmd file
</commit_message>
<xml_diff>
--- a/grain yield2.xlsx
+++ b/grain yield2.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raksha\Dropbox\Data for thesis\New analysis\Dryland\Yield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkt25\Desktop\Masters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A793E-2B84-461C-9743-32A3B1C762B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C009F81C-50A9-4267-8098-1DF4A6A66F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="18">
   <si>
     <t>location</t>
   </si>
@@ -93,30 +89,6 @@
   <si>
     <t>actual N (kg/ha)</t>
   </si>
-  <si>
-    <t>Average of yield (kg/ha)</t>
-  </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
-    <t>Column Labels</t>
-  </si>
-  <si>
-    <t>Einkorn Total</t>
-  </si>
-  <si>
-    <t>Emmer Total</t>
-  </si>
-  <si>
-    <t>Spelt Total</t>
-  </si>
-  <si>
-    <t>Wheat Total</t>
-  </si>
 </sst>
 </file>
 
@@ -157,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -172,8 +144,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,1459 +159,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Raksha" refreshedDate="44369.610470833337" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="106" xr:uid="{03D10565-CDF9-478F-AD44-60EADCDF5CDB}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J107" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields count="10">
-    <cacheField name="year" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2019" maxValue="2020" count="2">
-        <n v="2019"/>
-        <n v="2020"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="location" numFmtId="0">
-      <sharedItems count="2">
-        <s v="SAREC"/>
-        <s v="ShREC"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Season" numFmtId="0">
-      <sharedItems count="1">
-        <s v="Spring"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="crop" numFmtId="0">
-      <sharedItems count="4">
-        <s v="Einkorn"/>
-        <s v="Spelt"/>
-        <s v="Emmer"/>
-        <s v="Wheat"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Irrigation" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Plot" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="101" maxValue="342"/>
-    </cacheField>
-    <cacheField name="nitrogen" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="25" maxValue="80"/>
-    </cacheField>
-    <cacheField name="yield (kg/ha)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="85.855982602616479" maxValue="3175.9953773778188"/>
-    </cacheField>
-    <cacheField name="twt (kg)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="25.126349622573056" maxValue="29.331141192117251"/>
-    </cacheField>
-    <cacheField name="actual N (kg/ha)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="22.8990585793454" maxValue="92.013707239045132"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="106">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="101"/>
-    <n v="50"/>
-    <n v="140.86924965273599"/>
-    <n v="26.463946940738559"/>
-    <n v="55.386481503272833"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="102"/>
-    <n v="50"/>
-    <n v="401.71091436748804"/>
-    <n v="27.327945208453119"/>
-    <n v="57.865101879091036"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="103"/>
-    <n v="50"/>
-    <n v="774.23284335936012"/>
-    <n v="26.675146517291008"/>
-    <n v="55.386481503272833"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="104"/>
-    <n v="50"/>
-    <n v="811.21118252764052"/>
-    <n v="27.724744412884991"/>
-    <n v="55.386481503272833"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="105"/>
-    <n v="25"/>
-    <n v="767.26475355177308"/>
-    <n v="27.974343912446979"/>
-    <n v="29.772234317381596"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="106"/>
-    <n v="25"/>
-    <n v="142.83601055539199"/>
-    <n v="25.958347954446339"/>
-    <n v="29.772234317381596"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="107"/>
-    <n v="25"/>
-    <n v="869.88497037831553"/>
-    <n v="26.486346895827456"/>
-    <n v="29.772234317381596"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="108"/>
-    <n v="25"/>
-    <n v="361.64539171448473"/>
-    <n v="27.225545413761022"/>
-    <n v="22.8990585793454"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="109"/>
-    <n v="80"/>
-    <n v="342.66470285613178"/>
-    <n v="27.334345195621378"/>
-    <n v="88.972457492248338"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="110"/>
-    <n v="80"/>
-    <n v="1053.2619246504962"/>
-    <n v="28.323143213116929"/>
-    <n v="88.972457492248338"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="111"/>
-    <n v="80"/>
-    <n v="162.91757936752944"/>
-    <n v="26.476746915075072"/>
-    <n v="91.290686238372516"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="112"/>
-    <n v="80"/>
-    <n v="869.75843245259307"/>
-    <n v="26.780746305567231"/>
-    <n v="88.972457492248338"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="201"/>
-    <n v="25"/>
-    <n v="1131.6606992861068"/>
-    <n v="28.36474312971059"/>
-    <n v="28.006079879648887"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="202"/>
-    <n v="25"/>
-    <n v="85.855982602616479"/>
-    <n v="25.958347954446339"/>
-    <n v="28.006079879648887"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="203"/>
-    <n v="25"/>
-    <n v="726.95654879232018"/>
-    <n v="26.457546953570304"/>
-    <n v="25.651039939824443"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="204"/>
-    <n v="25"/>
-    <n v="295.88018068224"/>
-    <n v="27.66074454120243"/>
-    <n v="30.361119819473327"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="205"/>
-    <n v="50"/>
-    <n v="1073.5039602387694"/>
-    <n v="28.121543617316863"/>
-    <n v="54.846228746124176"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="206"/>
-    <n v="50"/>
-    <n v="594.34863711789183"/>
-    <n v="26.220747428344833"/>
-    <n v="57.164457492248346"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="207"/>
-    <n v="50"/>
-    <n v="336.97049619862594"/>
-    <n v="27.295945272611839"/>
-    <n v="54.846228746124176"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="208"/>
-    <n v="50"/>
-    <n v="178.73482008282357"/>
-    <n v="26.463946940738559"/>
-    <n v="57.164457492248346"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="209"/>
-    <n v="80"/>
-    <n v="920.76286771642594"/>
-    <n v="28.003143854704131"/>
-    <n v="88.391422524419625"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="210"/>
-    <n v="80"/>
-    <n v="376.82994280116708"/>
-    <n v="26.886346093843457"/>
-    <n v="88.391422524419625"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="211"/>
-    <n v="80"/>
-    <n v="697.22397073016487"/>
-    <n v="26.34554717812582"/>
-    <n v="90.699133786629432"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="212"/>
-    <n v="80"/>
-    <n v="123.62359912056"/>
-    <n v="26.476746915075072"/>
-    <n v="90.699133786629432"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="301"/>
-    <n v="80"/>
-    <n v="239.11318220327999"/>
-    <n v="26.476746915075072"/>
-    <n v="89.641138159363422"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="302"/>
-    <n v="80"/>
-    <n v="432.24971978496012"/>
-    <n v="27.167945529246719"/>
-    <n v="89.641138159363422"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="303"/>
-    <n v="80"/>
-    <n v="690.13332767808015"/>
-    <n v="27.100745663980032"/>
-    <n v="87.268569079681711"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="304"/>
-    <n v="80"/>
-    <n v="849.56772467952021"/>
-    <n v="26.265547338522623"/>
-    <n v="92.013707239045132"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="305"/>
-    <n v="50"/>
-    <n v="337.92528236543995"/>
-    <n v="27.24474537526579"/>
-    <n v="53.928560533967612"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="306"/>
-    <n v="50"/>
-    <n v="634.9756313554243"/>
-    <n v="27.039945785881599"/>
-    <n v="53.928560533967612"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="307"/>
-    <n v="50"/>
-    <n v="153.57869700095998"/>
-    <n v="26.463946940738559"/>
-    <n v="56.672747378623484"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="308"/>
-    <n v="50"/>
-    <n v="437.22016785216005"/>
-    <n v="25.452748968154111"/>
-    <n v="59.416934223279355"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="309"/>
-    <n v="25"/>
-    <n v="181.62901681435338"/>
-    <n v="25.958347954446339"/>
-    <n v="30.4628824277581"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="310"/>
-    <n v="25"/>
-    <n v="792.06632774744276"/>
-    <n v="26.799946267071999"/>
-    <n v="30.4628824277581"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="311"/>
-    <n v="25"/>
-    <n v="453.37794445579516"/>
-    <n v="27.289545285443584"/>
-    <n v="25.53544121387905"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="312"/>
-    <n v="25"/>
-    <n v="431.57950920246111"/>
-    <n v="25.30554926328422"/>
-    <n v="25.53544121387905"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="101"/>
-    <n v="80"/>
-    <n v="211.918487261184"/>
-    <n v="26.72634641463706"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="102"/>
-    <n v="80"/>
-    <n v="680.64425789833854"/>
-    <n v="27.545544772173823"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="103"/>
-    <n v="80"/>
-    <n v="1775.5217716164925"/>
-    <n v="28.105543649396221"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="104"/>
-    <n v="80"/>
-    <n v="1244.7957546393602"/>
-    <n v="27.295945272611839"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="105"/>
-    <n v="25"/>
-    <n v="146.27784213503998"/>
-    <n v="26.918346029684738"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="106"/>
-    <n v="25"/>
-    <n v="704.89616496343581"/>
-    <n v="27.40474505447219"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="107"/>
-    <n v="25"/>
-    <n v="912.31180489485462"/>
-    <n v="26.348747171709952"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="108"/>
-    <n v="25"/>
-    <n v="1514.2926769010526"/>
-    <n v="27.385545092967423"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="109"/>
-    <n v="50"/>
-    <n v="941.80172869329851"/>
-    <n v="26.342347184541698"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="110"/>
-    <n v="50"/>
-    <n v="697.88777624215106"/>
-    <n v="27.423945015976958"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="111"/>
-    <n v="50"/>
-    <n v="2417.6280771386755"/>
-    <n v="27.446344971065855"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="112"/>
-    <n v="50"/>
-    <n v="181.5819234115765"/>
-    <n v="26.534346799589375"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="201"/>
-    <n v="50"/>
-    <n v="2269.1670025956328"/>
-    <n v="27.996743867535873"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="202"/>
-    <n v="50"/>
-    <n v="743.830966723252"/>
-    <n v="27.48794488765952"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="203"/>
-    <n v="50"/>
-    <n v="720.69162603575353"/>
-    <n v="27.967943925278721"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="204"/>
-    <n v="50"/>
-    <n v="193.47648842947768"/>
-    <n v="26.534346799589375"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="205"/>
-    <n v="80"/>
-    <n v="1256.8499170410555"/>
-    <n v="26.259147351354368"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="206"/>
-    <n v="80"/>
-    <n v="2829.1623028518748"/>
-    <n v="28.188743482583551"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="207"/>
-    <n v="80"/>
-    <n v="357.34310223992475"/>
-    <n v="25.126349622573056"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="208"/>
-    <n v="80"/>
-    <n v="1231.5012925693234"/>
-    <n v="27.916744027932673"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="209"/>
-    <n v="25"/>
-    <n v="1120.1068786063915"/>
-    <n v="26.636746594281473"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="210"/>
-    <n v="25"/>
-    <n v="1432.6623950284802"/>
-    <n v="26.582346703351298"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="211"/>
-    <n v="25"/>
-    <n v="543.09682289016007"/>
-    <n v="26.463946940738559"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="212"/>
-    <n v="25"/>
-    <n v="1286.8496652690683"/>
-    <n v="27.391945080135681"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="301"/>
-    <n v="80"/>
-    <n v="702.46826476287993"/>
-    <n v="25.983947903119361"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="302"/>
-    <n v="80"/>
-    <n v="845.39988175104008"/>
-    <n v="27.711944438548478"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="303"/>
-    <n v="80"/>
-    <n v="2502.2593616204808"/>
-    <n v="28.697542462459904"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="304"/>
-    <n v="80"/>
-    <n v="405.42355970424006"/>
-    <n v="26.591946684103679"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="305"/>
-    <n v="50"/>
-    <n v="811.73737356495587"/>
-    <n v="27.839944181913598"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="306"/>
-    <n v="50"/>
-    <n v="732.78454780208438"/>
-    <n v="25.958347954446339"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="307"/>
-    <n v="50"/>
-    <n v="237.66890036736001"/>
-    <n v="26.534346799589375"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="308"/>
-    <n v="50"/>
-    <n v="927.55035509635479"/>
-    <n v="27.353545157126142"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="309"/>
-    <n v="25"/>
-    <n v="129.55599857857865"/>
-    <n v="26.918346029684738"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="310"/>
-    <n v="25"/>
-    <n v="748.553785262823"/>
-    <n v="26.2975472743639"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="311"/>
-    <n v="25"/>
-    <n v="864.4703928675483"/>
-    <n v="26.847946170833922"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="312"/>
-    <n v="25"/>
-    <n v="622.94030759885595"/>
-    <n v="27.187145490751487"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="131"/>
-    <n v="50"/>
-    <n v="591.11193017573055"/>
-    <n v="25.932748005773313"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="132"/>
-    <n v="50"/>
-    <n v="748.5983685734401"/>
-    <n v="26.905546055348221"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="133"/>
-    <n v="50"/>
-    <n v="1784.2047323576592"/>
-    <n v="28.2623433350185"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="135"/>
-    <n v="80"/>
-    <n v="849.81538936966751"/>
-    <n v="27.564744733678591"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="136"/>
-    <n v="80"/>
-    <n v="2135.6338515427706"/>
-    <n v="28.2623433350185"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="137"/>
-    <n v="80"/>
-    <n v="710.33063587866945"/>
-    <n v="26.489546889411582"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="138"/>
-    <n v="80"/>
-    <n v="1007.7547003436464"/>
-    <n v="27.206345452256258"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="139"/>
-    <n v="25"/>
-    <n v="772.14774253945257"/>
-    <n v="27.3599451442944"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="140"/>
-    <n v="25"/>
-    <n v="1008.3207910639833"/>
-    <n v="27.334345195621378"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="141"/>
-    <n v="25"/>
-    <n v="885.81875918309049"/>
-    <n v="26.918346029684738"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="142"/>
-    <n v="25"/>
-    <n v="2647.8327353035452"/>
-    <n v="28.76794232131072"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="231"/>
-    <n v="25"/>
-    <n v="767.39258048862303"/>
-    <n v="26.65594655578624"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="232"/>
-    <n v="25"/>
-    <n v="2334.4449125250694"/>
-    <n v="28.460742937234432"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="233"/>
-    <n v="25"/>
-    <n v="1386.214651424842"/>
-    <n v="27.3599451442944"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="234"/>
-    <n v="25"/>
-    <n v="833.3987584798989"/>
-    <n v="27.174345516414977"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="235"/>
-    <n v="50"/>
-    <n v="1285.1391533086987"/>
-    <n v="26.649546568617982"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="236"/>
-    <n v="50"/>
-    <n v="3175.9953773778188"/>
-    <n v="28.35194315537408"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="237"/>
-    <n v="50"/>
-    <n v="1340.644348437726"/>
-    <n v="27.193545477919741"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="238"/>
-    <n v="50"/>
-    <n v="1276.7610106477134"/>
-    <n v="28.118343623732738"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="239"/>
-    <n v="80"/>
-    <n v="806.79249462406744"/>
-    <n v="26.879946106675199"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="240"/>
-    <n v="80"/>
-    <n v="1082.3654572840423"/>
-    <n v="26.591946684103679"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="241"/>
-    <n v="80"/>
-    <n v="2918.5373177686233"/>
-    <n v="28.94074197485363"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="242"/>
-    <n v="80"/>
-    <n v="1304.9523285204882"/>
-    <n v="27.564744733678591"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="331"/>
-    <n v="80"/>
-    <n v="966.09042332685465"/>
-    <n v="27.295945272611839"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="333"/>
-    <n v="80"/>
-    <n v="788.11150085295151"/>
-    <n v="26.636746594281473"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="334"/>
-    <n v="80"/>
-    <n v="2293.7995988048842"/>
-    <n v="28.371143116878848"/>
-    <n v="89.600000000000009"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="335"/>
-    <n v="50"/>
-    <n v="925.67154589480435"/>
-    <n v="27.654344554034175"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="336"/>
-    <n v="50"/>
-    <n v="3050.0968011749055"/>
-    <n v="28.89594206467584"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="337"/>
-    <n v="50"/>
-    <n v="1673.8969605819048"/>
-    <n v="27.238345388097535"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="338"/>
-    <n v="50"/>
-    <n v="1227.2846816902736"/>
-    <n v="27.02714581154509"/>
-    <n v="56.000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <s v="Dryland"/>
-    <n v="339"/>
-    <n v="25"/>
-    <n v="1416.6986367149811"/>
-    <n v="27.55834474651034"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <s v="Dryland"/>
-    <n v="340"/>
-    <n v="25"/>
-    <n v="1257.4007080121937"/>
-    <n v="26.521546825252862"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <s v="Dryland"/>
-    <n v="341"/>
-    <n v="25"/>
-    <n v="3049.9835830308384"/>
-    <n v="29.331141192117251"/>
-    <n v="28.000000000000004"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Dryland"/>
-    <n v="342"/>
-    <n v="25"/>
-    <n v="1204.5278347327328"/>
-    <n v="27.001545862872064"/>
-    <n v="28.000000000000004"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F30EC43B-C602-4CBC-8281-82C2016C7091}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:N8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="3"/>
-    <field x="0"/>
-  </colFields>
-  <colItems count="13">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="default">
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of yield (kg/ha)" fld="7" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1906,233 +423,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C0D6CB-B704-48CF-B366-F86842D5036B}">
-  <dimension ref="A3:N8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>2019</v>
-      </c>
-      <c r="C5">
-        <v>2020</v>
-      </c>
-      <c r="E5">
-        <v>2019</v>
-      </c>
-      <c r="F5">
-        <v>2020</v>
-      </c>
-      <c r="H5">
-        <v>2019</v>
-      </c>
-      <c r="I5">
-        <v>2020</v>
-      </c>
-      <c r="K5">
-        <v>2019</v>
-      </c>
-      <c r="L5">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="6">
-        <v>156.57312637780564</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
-        <v>156.57312637780564</v>
-      </c>
-      <c r="E6" s="6">
-        <v>694.53031161830961</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6">
-        <v>694.53031161830961</v>
-      </c>
-      <c r="H6" s="6">
-        <v>371.02828613625923</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6">
-        <v>371.02828613625923</v>
-      </c>
-      <c r="K6" s="6">
-        <v>874.98229719468452</v>
-      </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6">
-        <v>874.98229719468452</v>
-      </c>
-      <c r="N6" s="6">
-        <v>524.27850533176468</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>267.37145833528234</v>
-      </c>
-      <c r="C7" s="6">
-        <v>954.99504520825258</v>
-      </c>
-      <c r="D7" s="6">
-        <v>611.18325177176746</v>
-      </c>
-      <c r="E7" s="6">
-        <v>968.45101831645422</v>
-      </c>
-      <c r="F7" s="6">
-        <v>1282.9347294447991</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1106.0376419351048</v>
-      </c>
-      <c r="H7" s="6">
-        <v>853.03729383321536</v>
-      </c>
-      <c r="I7" s="6">
-        <v>949.08254212917882</v>
-      </c>
-      <c r="J7" s="6">
-        <v>901.05991798119726</v>
-      </c>
-      <c r="K7" s="6">
-        <v>1793.9301689653876</v>
-      </c>
-      <c r="L7" s="6">
-        <v>2598.9476566540125</v>
-      </c>
-      <c r="M7" s="6">
-        <v>2196.4389128097</v>
-      </c>
-      <c r="N7" s="6">
-        <v>1206.4697108155665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6">
-        <v>211.97229235654405</v>
-      </c>
-      <c r="C8" s="6">
-        <v>954.99504520825258</v>
-      </c>
-      <c r="D8" s="6">
-        <v>459.64654330711352</v>
-      </c>
-      <c r="E8" s="6">
-        <v>831.49066496738192</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1282.9347294447991</v>
-      </c>
-      <c r="G8" s="6">
-        <v>957.89500302105853</v>
-      </c>
-      <c r="H8" s="6">
-        <v>612.03278998473741</v>
-      </c>
-      <c r="I8" s="6">
-        <v>949.08254212917882</v>
-      </c>
-      <c r="J8" s="6">
-        <v>724.38270736621791</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1334.4562330800359</v>
-      </c>
-      <c r="L8" s="6">
-        <v>2598.9476566540125</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1755.9533742713613</v>
-      </c>
-      <c r="N8" s="6">
-        <v>974.7821315946527</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
       <selection sqref="A1:J107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="7" width="8.85546875" style="2"/>
+    <col min="6" max="7" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2164,7 +467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2019</v>
       </c>
@@ -2196,7 +499,7 @@
         <v>55.386481503272833</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2019</v>
       </c>
@@ -2228,7 +531,7 @@
         <v>57.865101879091036</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2019</v>
       </c>
@@ -2260,7 +563,7 @@
         <v>55.386481503272833</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2019</v>
       </c>
@@ -2292,7 +595,7 @@
         <v>55.386481503272833</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2019</v>
       </c>
@@ -2324,7 +627,7 @@
         <v>29.772234317381596</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2019</v>
       </c>
@@ -2356,7 +659,7 @@
         <v>29.772234317381596</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2019</v>
       </c>
@@ -2388,7 +691,7 @@
         <v>29.772234317381596</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2019</v>
       </c>
@@ -2420,7 +723,7 @@
         <v>22.8990585793454</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2019</v>
       </c>
@@ -2452,7 +755,7 @@
         <v>88.972457492248338</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>2019</v>
       </c>
@@ -2484,7 +787,7 @@
         <v>88.972457492248338</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>2019</v>
       </c>
@@ -2516,7 +819,7 @@
         <v>91.290686238372516</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2019</v>
       </c>
@@ -2548,7 +851,7 @@
         <v>88.972457492248338</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2019</v>
       </c>
@@ -2580,7 +883,7 @@
         <v>28.006079879648887</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2019</v>
       </c>
@@ -2612,7 +915,7 @@
         <v>28.006079879648887</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2019</v>
       </c>
@@ -2644,7 +947,7 @@
         <v>25.651039939824443</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>2019</v>
       </c>
@@ -2676,7 +979,7 @@
         <v>30.361119819473327</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>2019</v>
       </c>
@@ -2708,7 +1011,7 @@
         <v>54.846228746124176</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>2019</v>
       </c>
@@ -2740,7 +1043,7 @@
         <v>57.164457492248346</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>2019</v>
       </c>
@@ -2772,7 +1075,7 @@
         <v>54.846228746124176</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2019</v>
       </c>
@@ -2804,7 +1107,7 @@
         <v>57.164457492248346</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>2019</v>
       </c>
@@ -2836,7 +1139,7 @@
         <v>88.391422524419625</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>2019</v>
       </c>
@@ -2868,7 +1171,7 @@
         <v>88.391422524419625</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>2019</v>
       </c>
@@ -2900,7 +1203,7 @@
         <v>90.699133786629432</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>2019</v>
       </c>
@@ -2932,7 +1235,7 @@
         <v>90.699133786629432</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>2019</v>
       </c>
@@ -2964,7 +1267,7 @@
         <v>89.641138159363422</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>2019</v>
       </c>
@@ -2996,7 +1299,7 @@
         <v>89.641138159363422</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>2019</v>
       </c>
@@ -3028,7 +1331,7 @@
         <v>87.268569079681711</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>2019</v>
       </c>
@@ -3060,7 +1363,7 @@
         <v>92.013707239045132</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>2019</v>
       </c>
@@ -3092,7 +1395,7 @@
         <v>53.928560533967612</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>2019</v>
       </c>
@@ -3124,7 +1427,7 @@
         <v>53.928560533967612</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>2019</v>
       </c>
@@ -3156,7 +1459,7 @@
         <v>56.672747378623484</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>2019</v>
       </c>
@@ -3188,7 +1491,7 @@
         <v>59.416934223279355</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>2019</v>
       </c>
@@ -3220,7 +1523,7 @@
         <v>30.4628824277581</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>2019</v>
       </c>
@@ -3252,7 +1555,7 @@
         <v>30.4628824277581</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>2019</v>
       </c>
@@ -3284,7 +1587,7 @@
         <v>25.53544121387905</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>2019</v>
       </c>
@@ -3316,7 +1619,7 @@
         <v>25.53544121387905</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>2019</v>
       </c>
@@ -3349,7 +1652,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>2019</v>
       </c>
@@ -3382,7 +1685,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>2019</v>
       </c>
@@ -3415,7 +1718,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>2019</v>
       </c>
@@ -3448,7 +1751,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>2019</v>
       </c>
@@ -3481,7 +1784,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>2019</v>
       </c>
@@ -3514,7 +1817,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>2019</v>
       </c>
@@ -3547,7 +1850,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>2019</v>
       </c>
@@ -3580,7 +1883,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>2019</v>
       </c>
@@ -3613,7 +1916,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>2019</v>
       </c>
@@ -3646,7 +1949,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>2019</v>
       </c>
@@ -3679,7 +1982,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>2019</v>
       </c>
@@ -3712,7 +2015,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>2019</v>
       </c>
@@ -3745,7 +2048,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2019</v>
       </c>
@@ -3778,7 +2081,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>2019</v>
       </c>
@@ -3811,7 +2114,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>2019</v>
       </c>
@@ -3844,7 +2147,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>2019</v>
       </c>
@@ -3877,7 +2180,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2019</v>
       </c>
@@ -3910,7 +2213,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2019</v>
       </c>
@@ -3943,7 +2246,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2019</v>
       </c>
@@ -3976,7 +2279,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>2019</v>
       </c>
@@ -4009,7 +2312,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>2019</v>
       </c>
@@ -4042,7 +2345,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>2019</v>
       </c>
@@ -4075,7 +2378,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>2019</v>
       </c>
@@ -4108,7 +2411,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>2019</v>
       </c>
@@ -4141,7 +2444,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>2019</v>
       </c>
@@ -4174,7 +2477,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>2019</v>
       </c>
@@ -4207,7 +2510,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>2019</v>
       </c>
@@ -4240,7 +2543,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>2019</v>
       </c>
@@ -4273,7 +2576,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>2019</v>
       </c>
@@ -4306,7 +2609,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>2019</v>
       </c>
@@ -4339,7 +2642,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>2019</v>
       </c>
@@ -4372,7 +2675,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>2019</v>
       </c>
@@ -4405,7 +2708,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>2019</v>
       </c>
@@ -4438,7 +2741,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>2019</v>
       </c>
@@ -4471,7 +2774,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>2019</v>
       </c>
@@ -4504,7 +2807,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>2020</v>
       </c>
@@ -4537,7 +2840,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>2020</v>
       </c>
@@ -4570,7 +2873,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>2020</v>
       </c>
@@ -4603,7 +2906,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>2020</v>
       </c>
@@ -4636,7 +2939,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>2020</v>
       </c>
@@ -4669,7 +2972,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>2020</v>
       </c>
@@ -4702,7 +3005,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>2020</v>
       </c>
@@ -4735,7 +3038,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>2020</v>
       </c>
@@ -4768,7 +3071,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>2020</v>
       </c>
@@ -4801,7 +3104,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>2020</v>
       </c>
@@ -4834,7 +3137,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>2020</v>
       </c>
@@ -4867,7 +3170,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>2020</v>
       </c>
@@ -4900,7 +3203,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>2020</v>
       </c>
@@ -4933,7 +3236,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>2020</v>
       </c>
@@ -4966,7 +3269,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>2020</v>
       </c>
@@ -4999,7 +3302,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>2020</v>
       </c>
@@ -5032,7 +3335,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>2020</v>
       </c>
@@ -5065,7 +3368,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>2020</v>
       </c>
@@ -5098,7 +3401,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>2020</v>
       </c>
@@ -5131,7 +3434,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>2020</v>
       </c>
@@ -5164,7 +3467,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>2020</v>
       </c>
@@ -5197,7 +3500,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>2020</v>
       </c>
@@ -5230,7 +3533,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>2020</v>
       </c>
@@ -5263,7 +3566,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>2020</v>
       </c>
@@ -5296,7 +3599,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>2020</v>
       </c>
@@ -5329,7 +3632,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>2020</v>
       </c>
@@ -5362,7 +3665,7 @@
         <v>89.600000000000009</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>2020</v>
       </c>
@@ -5395,7 +3698,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>2020</v>
       </c>
@@ -5428,7 +3731,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>2020</v>
       </c>
@@ -5461,7 +3764,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>2020</v>
       </c>
@@ -5494,7 +3797,7 @@
         <v>56.000000000000007</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>2020</v>
       </c>
@@ -5527,7 +3830,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>2020</v>
       </c>
@@ -5560,7 +3863,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>2020</v>
       </c>
@@ -5593,7 +3896,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>2020</v>
       </c>

</xml_diff>